<commit_message>
update ai_type_list excel file
</commit_message>
<xml_diff>
--- a/database/excel_tables/individual_tables/ai_type_list.xlsx
+++ b/database/excel_tables/individual_tables/ai_type_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ai_type</t>
   </si>
@@ -40,9 +40,6 @@
     <t>explainable ai</t>
   </si>
   <si>
-    <t>feature selection and dimensionality reduction</t>
-  </si>
-  <si>
     <t>fuzzy logic</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>llm</t>
   </si>
   <si>
-    <t>local learning</t>
-  </si>
-  <si>
     <t>metaheuristics</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>multi-criteria decision making ai</t>
   </si>
   <si>
-    <t>neural networks</t>
-  </si>
-  <si>
     <t>nlp</t>
   </si>
   <si>
@@ -88,7 +79,7 @@
     <t>overall</t>
   </si>
   <si>
-    <t>probabilistic models</t>
+    <t>probabilistic reasoning</t>
   </si>
   <si>
     <t>reinforcement learning</t>
@@ -100,9 +91,6 @@
     <t>spatio-temporal ai</t>
   </si>
   <si>
-    <t>statistical and probabilistic models</t>
-  </si>
-  <si>
     <t>supervised machine learning</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
   </si>
   <si>
     <t>symbolic ai</t>
-  </si>
-  <si>
-    <t>time series analysis</t>
   </si>
   <si>
     <t>unspecified</t>
@@ -479,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -640,31 +625,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>